<commit_message>
Updated report storagefolder staructure
</commit_message>
<xml_diff>
--- a/example_urls.xlsx
+++ b/example_urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TrigentSales\SiteSenseAIEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94AAE1F-E240-424B-AC9A-4BCF022CA32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D7536F-EE92-4227-80D3-1E386B1FD630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3C86CCD8-EA5F-4B99-A5DB-67613E73B2DB}"/>
   </bookViews>
@@ -36,9 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>url</t>
+  </si>
+  <si>
+    <t>https://www.odiware.com/</t>
+  </si>
+  <si>
+    <t>https://indianmusic.in/</t>
   </si>
   <si>
     <t>https://staging16.trigent.com/</t>
@@ -424,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38AC088-1BB7-4BD1-9090-C5EB208AF5F7}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,11 +452,20 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{7AA67DED-8A7C-4512-A01C-7A3C9132664C}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{35CCB518-1871-4523-8730-A01B2C47E478}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{306A3CE7-8E2F-4FD2-8F6F-3AE8AA5E6078}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Browser Manager and site analyzer
</commit_message>
<xml_diff>
--- a/example_urls.xlsx
+++ b/example_urls.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TrigentSales\SiteSenseAIEngine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartAutomation\SiteSenseAIEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D7536F-EE92-4227-80D3-1E386B1FD630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC0E835-4110-4E9B-8CF0-DC3653557280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3C86CCD8-EA5F-4B99-A5DB-67613E73B2DB}"/>
   </bookViews>
@@ -36,18 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>url</t>
   </si>
   <si>
-    <t>https://www.odiware.com/</t>
-  </si>
-  <si>
-    <t>https://indianmusic.in/</t>
-  </si>
-  <si>
-    <t>https://staging16.trigent.com/</t>
+    <t>https://www.trigent.com/</t>
   </si>
 </sst>
 </file>
@@ -433,7 +427,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,32 +446,25 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{7AA67DED-8A7C-4512-A01C-7A3C9132664C}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{35CCB518-1871-4523-8730-A01B2C47E478}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{306A3CE7-8E2F-4FD2-8F6F-3AE8AA5E6078}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="0fa9324a-d92c-4773-ad72-0d40e8b32217" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -714,17 +701,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="0fa9324a-d92c-4773-ad72-0d40e8b32217" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{329F615B-EEB6-4640-8E71-160F0E4594FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2C005F-462F-47B6-B9AE-1E929510F981}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="ffb3be80-777f-49b2-871e-bd1d3e941119"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0fa9324a-d92c-4773-ad72-0d40e8b32217"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -749,18 +746,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2C005F-462F-47B6-B9AE-1E929510F981}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{329F615B-EEB6-4640-8E71-160F0E4594FA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="ffb3be80-777f-49b2-871e-bd1d3e941119"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0fa9324a-d92c-4773-ad72-0d40e8b32217"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added smart wait feature
</commit_message>
<xml_diff>
--- a/example_urls.xlsx
+++ b/example_urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartAutomation\SiteSenseAIEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC0E835-4110-4E9B-8CF0-DC3653557280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A7272F-3A62-43E4-AEC4-8C6E05EC6C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3C86CCD8-EA5F-4B99-A5DB-67613E73B2DB}"/>
   </bookViews>
@@ -36,12 +36,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>url</t>
   </si>
   <si>
-    <t>https://www.trigent.com/</t>
+    <t>https://www.wineenthusiast.com/</t>
+  </si>
+  <si>
+    <t>https://www.loopnet.com/</t>
+  </si>
+  <si>
+    <t>https://www.hannaandersson.com/</t>
+  </si>
+  <si>
+    <t>https://www.foco.com/</t>
+  </si>
+  <si>
+    <t>https://www.designrush.com/</t>
   </si>
 </sst>
 </file>
@@ -424,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38AC088-1BB7-4BD1-9090-C5EB208AF5F7}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,25 +458,44 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{7AA67DED-8A7C-4512-A01C-7A3C9132664C}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{F6370AE1-0ABB-405F-8D3C-86CA34083DEA}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{E835B678-9D5C-4D25-A5B9-33D543B7680F}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{0D0CE18F-8025-40F5-9EC6-EB20B3E51666}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{1CB7E317-3D54-4856-8D16-2C5CB648B433}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="0fa9324a-d92c-4773-ad72-0d40e8b32217" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -701,27 +732,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="0fa9324a-d92c-4773-ad72-0d40e8b32217" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2C005F-462F-47B6-B9AE-1E929510F981}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{329F615B-EEB6-4640-8E71-160F0E4594FA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="ffb3be80-777f-49b2-871e-bd1d3e941119"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0fa9324a-d92c-4773-ad72-0d40e8b32217"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -746,9 +767,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{329F615B-EEB6-4640-8E71-160F0E4594FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2C005F-462F-47B6-B9AE-1E929510F981}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="ffb3be80-777f-49b2-871e-bd1d3e941119"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0fa9324a-d92c-4773-ad72-0d40e8b32217"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Redesign the report UI
</commit_message>
<xml_diff>
--- a/example_urls.xlsx
+++ b/example_urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartAutomation\SiteSenseAIEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A7272F-3A62-43E4-AEC4-8C6E05EC6C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9F387C-F55C-4070-94CA-A7E7225F4A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3C86CCD8-EA5F-4B99-A5DB-67613E73B2DB}"/>
   </bookViews>
@@ -36,24 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>url</t>
   </si>
   <si>
     <t>https://www.wineenthusiast.com/</t>
-  </si>
-  <si>
-    <t>https://www.loopnet.com/</t>
-  </si>
-  <si>
-    <t>https://www.hannaandersson.com/</t>
-  </si>
-  <si>
-    <t>https://www.foco.com/</t>
-  </si>
-  <si>
-    <t>https://www.designrush.com/</t>
   </si>
 </sst>
 </file>
@@ -439,7 +427,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,32 +446,20 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A5" s="1"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A6" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{7AA67DED-8A7C-4512-A01C-7A3C9132664C}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{F6370AE1-0ABB-405F-8D3C-86CA34083DEA}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{E835B678-9D5C-4D25-A5B9-33D543B7680F}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{0D0CE18F-8025-40F5-9EC6-EB20B3E51666}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{1CB7E317-3D54-4856-8D16-2C5CB648B433}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Redesign the report UI Report name
</commit_message>
<xml_diff>
--- a/example_urls.xlsx
+++ b/example_urls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartAutomation\SiteSenseAIEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9F387C-F55C-4070-94CA-A7E7225F4A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40C29AC-CD6C-4AAA-9B40-AFB0D46F868A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3C86CCD8-EA5F-4B99-A5DB-67613E73B2DB}"/>
+    <workbookView xWindow="1284" yWindow="1044" windowWidth="21720" windowHeight="11088" xr2:uid="{3C86CCD8-EA5F-4B99-A5DB-67613E73B2DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,19 +36,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>url</t>
+    <t>CompanyName</t>
   </si>
   <si>
-    <t>https://www.wineenthusiast.com/</t>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://www.trigent.com/</t>
+  </si>
+  <si>
+    <t>Trigent Software Ltd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,13 +70,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -86,9 +106,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -424,57 +445,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38AC088-1BB7-4BD1-9090-C5EB208AF5F7}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="56.21875" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" customWidth="1"/>
+    <col min="2" max="2" width="56.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="1"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{7AA67DED-8A7C-4512-A01C-7A3C9132664C}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{7AA67DED-8A7C-4512-A01C-7A3C9132664C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BC55A24CF65DCC4187A3367C741B7A96" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0a3770f1695041ea4eaa4abe8180211c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ffb3be80-777f-49b2-871e-bd1d3e941119" xmlns:ns4="0fa9324a-d92c-4773-ad72-0d40e8b32217" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f32754687f6322110bda802cf804242" ns3:_="" ns4:_="">
     <xsd:import namespace="ffb3be80-777f-49b2-871e-bd1d3e941119"/>
@@ -707,6 +726,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -716,14 +744,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{329F615B-EEB6-4640-8E71-160F0E4594FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D95F558-DF4F-43DB-8116-74C86C3E2DC9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -742,6 +762,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{329F615B-EEB6-4640-8E71-160F0E4594FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2C005F-462F-47B6-B9AE-1E929510F981}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Update test runner and example URLs
</commit_message>
<xml_diff>
--- a/example_urls.xlsx
+++ b/example_urls.xlsx
@@ -1,85 +1,198 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartAutomation\SiteSenseAIEngine\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40C29AC-CD6C-4AAA-9B40-AFB0D46F868A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="1284" yWindow="1044" windowWidth="21720" windowHeight="11088" xr2:uid="{3C86CCD8-EA5F-4B99-A5DB-67613E73B2DB}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>CompanyName</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>https://www.trigent.com/</t>
-  </si>
-  <si>
-    <t>Trigent Software Ltd</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+  <si>
+    <t xml:space="preserve">CompanyName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eakes Office Solutions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://eakes.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ShipOffers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.shipoffers.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FlexTG Sacramento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.flextg.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SeekWell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.seekwell.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Kent Companies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://thekentcompanies.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint Mart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.sprintmart.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colorvision International, Inc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://colorvisionint.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crosby's Stores (Reid Stores, Inc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.crosbysstores.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meade Tractor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://meadetractor.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family Leisure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.familyleisure.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BlueWave Express Car Wash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bluewaveexpress.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Computers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.centralcomputer.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aqua Systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.aquasystems.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diane &amp; Geordi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dianeandgeordi.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOPP Business Solutions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://toppcopy.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balls Food Stores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ballsfoods.com/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
-      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,13 +201,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.499984740745262"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="3" tint="0.4999"/>
+        <bgColor rgb="FF467886"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF93C47D"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -102,222 +221,228 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="21">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+  <cellXfs count="7">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF93C47D"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF467886"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF4E95D9"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="0e2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="e8e8e8"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="e97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="196b24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="0f9ed5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="a02b93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="4ea72e"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="96607d"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
                 <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
                 <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
                 <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
                 <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
                 <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
               </a:schemeClr>
@@ -325,33 +450,24 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
                 <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
@@ -364,13 +480,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -380,15 +490,13 @@
         <a:solidFill>
           <a:schemeClr val="phClr">
             <a:tint val="95000"/>
-            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="93000"/>
-                <a:satMod val="150000"/>
                 <a:shade val="98000"/>
                 <a:lumMod val="102000"/>
               </a:schemeClr>
@@ -396,7 +504,6 @@
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:tint val="98000"/>
-                <a:satMod val="130000"/>
                 <a:shade val="90000"/>
                 <a:lumMod val="103000"/>
               </a:schemeClr>
@@ -404,92 +511,183 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="63000"/>
-                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38AC088-1BB7-4BD1-9090-C5EB208AF5F7}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="14.25" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" customWidth="1"/>
-    <col min="2" max="2" width="56.21875" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{7AA67DED-8A7C-4512-A01C-7A3C9132664C}"/>
+    <hyperlink ref="B17" r:id="rId1" display="https://ballsfoods.com/"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 

</xml_diff>